<commit_message>
new tc with Data driven testng approach
</commit_message>
<xml_diff>
--- a/src/test/java/com/testData/LoginData.xlsx
+++ b/src/test/java/com/testData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sneharoy/eclipse-workspace/InetBankingV1/src/test/java/com/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B3CAE32-742D-764E-8CBD-EF5343C1D43F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3117F7F0-429E-EC4A-9509-7D61B5D6AD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{0880F767-000E-9E47-8B70-8168F01619E2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>qAbUzyj</t>
-  </si>
-  <si>
-    <t>mngr137319</t>
-  </si>
-  <si>
-    <t>bAdYvyb</t>
   </si>
   <si>
     <t>mngr112909</t>
@@ -459,7 +453,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,10 +472,10 @@
     </row>
     <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -494,10 +488,10 @@
     </row>
     <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
@@ -510,10 +504,10 @@
     </row>
     <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>